<commit_message>
Added some JUnit tests.
</commit_message>
<xml_diff>
--- a/doc/test-plan.xlsx
+++ b/doc/test-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertmoller/Documents/Hobby/Code/University/Assignment/New/Contacts/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1420C0-C574-C046-9A38-B57F94912BEE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B72616D-3A81-B747-85D6-05D68F34771B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{CBFCEDE9-383C-6A40-9CD9-DE0218603E41}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -202,6 +202,63 @@
   </si>
   <si>
     <t>Context menu shows up and functions properly.</t>
+  </si>
+  <si>
+    <t>The field being at the top should of the list of a contacts fields should only have 1 line above</t>
+  </si>
+  <si>
+    <t>A contact does not have any associated numbers.</t>
+  </si>
+  <si>
+    <t>The top field has double lines and a longer distance to the start of the list than the number field would have.</t>
+  </si>
+  <si>
+    <t>Information shows up correctly.</t>
+  </si>
+  <si>
+    <t>Information copies successfully.</t>
+  </si>
+  <si>
+    <t>Information saves correctly</t>
+  </si>
+  <si>
+    <t>Information saves correctly.</t>
+  </si>
+  <si>
+    <t>Information is deleted correctly.</t>
+  </si>
+  <si>
+    <t>Application quits.</t>
+  </si>
+  <si>
+    <t>Application minimises.</t>
+  </si>
+  <si>
+    <t>Application maximises.</t>
+  </si>
+  <si>
+    <t>Windows minimum size is set and functions correctly.</t>
+  </si>
+  <si>
+    <t>Filepicker pops up and uploads pictures correctly</t>
+  </si>
+  <si>
+    <t>Filepicker has a file filter for pictures.</t>
+  </si>
+  <si>
+    <t>Profile picture is deleted correctly.</t>
+  </si>
+  <si>
+    <t>User is prohibited of selected a different contact or leaving edit mode.</t>
+  </si>
+  <si>
+    <t>Field is added and focus is set.</t>
+  </si>
+  <si>
+    <t>Profile picture is deleted.</t>
+  </si>
+  <si>
+    <t>Contact is deleted.</t>
   </si>
 </sst>
 </file>
@@ -673,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1A66C9-500D-D94A-91FB-E8966283DEF3}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="56" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -684,7 +741,7 @@
     <col min="3" max="3" width="56.83203125" style="9" customWidth="1"/>
     <col min="4" max="4" width="74.6640625" style="8" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="5" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" style="2"/>
     <col min="8" max="8" width="7.5" style="4"/>
     <col min="9" max="16384" width="7.5" style="2"/>
@@ -874,6 +931,9 @@
       <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="D9" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="E9" s="1" t="str">
         <f>IF(F9=1,"Success",IF(F9="","","Failed"))</f>
         <v>Success</v>
@@ -893,6 +953,9 @@
       <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="D10" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="E10" s="1" t="str">
         <f>IF(F10=1,"Success",IF(F10="","","Failed"))</f>
         <v>Success</v>
@@ -912,6 +975,9 @@
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="D11" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="E11" s="1" t="str">
         <f>IF(F11=1,"Success",IF(F11="","","Failed"))</f>
         <v>Success</v>
@@ -931,6 +997,9 @@
       <c r="C12" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="D12" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="E12" s="1" t="str">
         <f>IF(F12=1,"Success",IF(F12="","","Failed"))</f>
         <v>Success</v>
@@ -950,6 +1019,9 @@
       <c r="C13" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="D13" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="E13" s="1" t="str">
         <f>IF(F13=1,"Success",IF(F13="","","Failed"))</f>
         <v>Success</v>
@@ -969,6 +1041,9 @@
       <c r="C14" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="D14" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="E14" s="1" t="str">
         <f>IF(F14=1,"Success",IF(F14="","","Failed"))</f>
         <v>Success</v>
@@ -988,6 +1063,9 @@
       <c r="C15" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="D15" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="E15" s="1" t="str">
         <f>IF(F15=1,"Success",IF(F15="","","Failed"))</f>
         <v>Success</v>
@@ -1007,6 +1085,9 @@
       <c r="C16" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="D16" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="E16" s="1" t="str">
         <f>IF(F16=1,"Success",IF(F16="","","Failed"))</f>
         <v>Success</v>
@@ -1026,6 +1107,9 @@
       <c r="C17" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="D17" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="E17" s="1" t="str">
         <f>IF(F17=1,"Success",IF(F17="","","Failed"))</f>
         <v>Success</v>
@@ -1045,6 +1129,9 @@
       <c r="C18" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="D18" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="E18" s="1" t="str">
         <f>IF(F18=1,"Success",IF(F18="","","Failed"))</f>
         <v>Success</v>
@@ -1064,6 +1151,9 @@
       <c r="C19" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="D19" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="E19" s="1" t="str">
         <f>IF(F19=1,"Success",IF(F19="","","Failed"))</f>
         <v>Success</v>
@@ -1083,6 +1173,9 @@
       <c r="C20" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="D20" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="E20" s="1" t="str">
         <f>IF(F20=1,"Success",IF(F20="","","Failed"))</f>
         <v>Success</v>
@@ -1102,6 +1195,9 @@
       <c r="C21" s="8" t="s">
         <v>44</v>
       </c>
+      <c r="D21" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="E21" s="1" t="str">
         <f>IF(F21=1,"Success",IF(F21="","","Failed"))</f>
         <v>Success</v>
@@ -1121,6 +1217,9 @@
       <c r="C22" s="8" t="s">
         <v>45</v>
       </c>
+      <c r="D22" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="E22" s="1" t="str">
         <f>IF(F22=1,"Success",IF(F22="","","Failed"))</f>
         <v>Success</v>
@@ -1140,6 +1239,9 @@
       <c r="C23" s="8" t="s">
         <v>49</v>
       </c>
+      <c r="D23" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="E23" s="1" t="str">
         <f>IF(F23=1,"Success",IF(F23="","","Failed"))</f>
         <v>Success</v>
@@ -1159,7 +1261,9 @@
       <c r="C24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="E24" s="1" t="str">
         <f>IF(F24=1,"Success",IF(F24="","","Failed"))</f>
         <v>Success</v>
@@ -1179,6 +1283,9 @@
       <c r="C25" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="D25" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="E25" s="1" t="str">
         <f>IF(F25=1,"Success",IF(F25="","","Failed"))</f>
         <v>Success</v>
@@ -1192,19 +1299,21 @@
       <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="e">
-        <f>-----w</f>
-        <v>#NAME?</v>
+      <c r="B26" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="E26" s="1" t="str">
         <f>IF(F26=1,"Success",IF(F26="","","Failed"))</f>
-        <v>Success</v>
+        <v>Failed</v>
       </c>
       <c r="F26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="2"/>
     </row>

</xml_diff>